<commit_message>
Fixed missing department/region leaders
</commit_message>
<xml_diff>
--- a/output/PA73405 - Attrition by Job 2009 - Finance - 2019-02-17.xlsx
+++ b/output/PA73405 - Attrition by Job 2009 - Finance - 2019-02-17.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve">year</t>
   </si>
@@ -40,6 +40,18 @@
   </si>
   <si>
     <t xml:space="preserve">30.8%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department Leader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.0%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regional Leader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.4%</t>
   </si>
   <si>
     <t xml:space="preserve">Product Manager</t>
@@ -140,8 +152,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F6" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:F6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:F8" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
     <tableColumn id="1" name="year"/>
     <tableColumn id="2" name="job_name"/>
@@ -497,13 +509,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -517,13 +529,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -537,13 +549,13 @@
         <v>13</v>
       </c>
       <c r="C5" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E5" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -557,16 +569,56 @@
         <v>15</v>
       </c>
       <c r="C6" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="n">
+        <v>13</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="n">
+        <v>16</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -591,37 +643,37 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>